<commit_message>
(v1.3.0.9012) data sets vignette update
</commit_message>
<xml_diff>
--- a/data-raw/antivirals.xlsx
+++ b/data-raw/antivirals.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="297">
   <si>
     <t xml:space="preserve">atc</t>
   </si>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">J05AF06</t>
   </si>
   <si>
-    <t xml:space="preserve">abacavir</t>
+    <t xml:space="preserve">Abacavir</t>
   </si>
   <si>
     <t xml:space="preserve">Nucleoside and nucleotide reverse transcriptase inhibitors</t>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">J05AB01</t>
   </si>
   <si>
-    <t xml:space="preserve">aciclovir</t>
+    <t xml:space="preserve">Aciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">Nucleosides and nucleotides excl. reverse transcriptase inhibitors</t>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">J05AF08</t>
   </si>
   <si>
-    <t xml:space="preserve">adefovir dipivoxil</t>
+    <t xml:space="preserve">Adefovir dipivoxil</t>
   </si>
   <si>
     <t xml:space="preserve">c("Adefovir di ester", "Adefovir dipivoxil", "Adefovir Dipivoxil", "Adefovir dipivoxyl", "Adefovir pivoxil", "Adefovirdipivoxl", "Bisadenine", "BISADENINE", "BisPMEA", "Hepsera", "Preveon", "YouHeDing")</t>
@@ -83,7 +83,7 @@
     <t xml:space="preserve">J05AE05</t>
   </si>
   <si>
-    <t xml:space="preserve">amprenavir</t>
+    <t xml:space="preserve">Amprenavir</t>
   </si>
   <si>
     <t xml:space="preserve">Protease inhibitors</t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">J05AP06</t>
   </si>
   <si>
-    <t xml:space="preserve">asunaprevir</t>
+    <t xml:space="preserve">Asunaprevir</t>
   </si>
   <si>
     <t xml:space="preserve">Antivirals for treatment of HCV infections</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">J05AE08</t>
   </si>
   <si>
-    <t xml:space="preserve">atazanavir</t>
+    <t xml:space="preserve">Atazanavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Atazanavir", "Atazanavir Base", "Latazanavir", "Reyataz", "Zrivada")</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">J05AR15</t>
   </si>
   <si>
-    <t xml:space="preserve">atazanavir and cobicistat</t>
+    <t xml:space="preserve">Atazanavir and cobicistat</t>
   </si>
   <si>
     <t xml:space="preserve">Antivirals for treatment of HIV infections, combinations</t>
@@ -128,13 +128,13 @@
     <t xml:space="preserve">J05AR23</t>
   </si>
   <si>
-    <t xml:space="preserve">atazanavir and ritonavir</t>
+    <t xml:space="preserve">Atazanavir and ritonavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP03</t>
   </si>
   <si>
-    <t xml:space="preserve">boceprevir</t>
+    <t xml:space="preserve">Boceprevir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Bocepravir", "Boceprevir", "Victrelis")</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">J05AB15</t>
   </si>
   <si>
-    <t xml:space="preserve">brivudine</t>
+    <t xml:space="preserve">Brivudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Bridic", "Brivox", "Brivudin", "Brivudina", "Brivudine", "Brivudinum", "BrVdUrd", "Helpin", "Zerpex", "Zostex")</t>
@@ -152,7 +152,7 @@
     <t xml:space="preserve">J05AB12</t>
   </si>
   <si>
-    <t xml:space="preserve">cidofovir</t>
+    <t xml:space="preserve">Cidofovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Cidofovir", "Cidofovir anhydrous", "Cidofovir gel", "Cidofovirum", "Forvade", "Vistide")</t>
@@ -161,7 +161,7 @@
     <t xml:space="preserve">J05AF12</t>
   </si>
   <si>
-    <t xml:space="preserve">clevudine</t>
+    <t xml:space="preserve">Clevudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Clevudine", "Levovir", "Revovir")</t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">J05AP07</t>
   </si>
   <si>
-    <t xml:space="preserve">daclatasvir</t>
+    <t xml:space="preserve">Daclatasvir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Daclatasvir", "Daklinza")</t>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">J05AE10</t>
   </si>
   <si>
-    <t xml:space="preserve">darunavir</t>
+    <t xml:space="preserve">Darunavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Darunavir", "Darunavirum", "Prezista", "Prezista Naive")</t>
@@ -188,28 +188,25 @@
     <t xml:space="preserve">J05AR14</t>
   </si>
   <si>
-    <t xml:space="preserve">darunavir and cobicistat</t>
+    <t xml:space="preserve">Darunavir and cobicistat</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP09</t>
   </si>
   <si>
-    <t xml:space="preserve">dasabuvir</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dasabuvir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP52</t>
   </si>
   <si>
-    <t xml:space="preserve">dasabuvir, ombitasvir, paritaprevir and ritonavir</t>
+    <t xml:space="preserve">Dasabuvir, ombitasvir, paritaprevir and ritonavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG02</t>
   </si>
   <si>
-    <t xml:space="preserve">delavirdine</t>
+    <t xml:space="preserve">Delavirdine</t>
   </si>
   <si>
     <t xml:space="preserve">Non-nucleoside reverse transcriptase inhibitors</t>
@@ -221,7 +218,7 @@
     <t xml:space="preserve">J05AF02</t>
   </si>
   <si>
-    <t xml:space="preserve">didanosine</t>
+    <t xml:space="preserve">Didanosine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Didanosina", "Didanosine", "Didanosinum", "Dideoxyinosine", "DIDEOXYINOSINE", "Hypoxanthine ddN", "Videx", "Videx EC")</t>
@@ -230,7 +227,7 @@
     <t xml:space="preserve">J05AX12</t>
   </si>
   <si>
-    <t xml:space="preserve">dolutegravir</t>
+    <t xml:space="preserve">Dolutegravir</t>
   </si>
   <si>
     <t xml:space="preserve">Other antivirals</t>
@@ -242,13 +239,13 @@
     <t xml:space="preserve">J05AR21</t>
   </si>
   <si>
-    <t xml:space="preserve">dolutegravir and rilpivirine</t>
+    <t xml:space="preserve">Dolutegravir and rilpivirine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG06</t>
   </si>
   <si>
-    <t xml:space="preserve">doravirine</t>
+    <t xml:space="preserve">Doravirine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Doravirine", "Pifeltro")</t>
@@ -257,7 +254,7 @@
     <t xml:space="preserve">J05AG03</t>
   </si>
   <si>
-    <t xml:space="preserve">efavirenz</t>
+    <t xml:space="preserve">Efavirenz</t>
   </si>
   <si>
     <t xml:space="preserve">c("Efavirenz", "Efavirenzum", "Eravirenz", "Stocrin", "Strocin", "Sustiva")</t>
@@ -266,13 +263,13 @@
     <t xml:space="preserve">J05AP54</t>
   </si>
   <si>
-    <t xml:space="preserve">elbasvir and grazoprevir</t>
+    <t xml:space="preserve">Elbasvir and grazoprevir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX11</t>
   </si>
   <si>
-    <t xml:space="preserve">elvitegravir</t>
+    <t xml:space="preserve">Elvitegravir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Elvitegravir", "Vitekta")</t>
@@ -281,7 +278,7 @@
     <t xml:space="preserve">J05AF09</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine</t>
+    <t xml:space="preserve">Emtricitabine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Coviracil", "Emtricitabin", "Emtricitabina", "Emtricitabine", "Emtricitabinum", "Emtritabine", "Emtriva", "Racivir")</t>
@@ -290,55 +287,55 @@
     <t xml:space="preserve">J05AR17</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine and tenofovir alafenamide</t>
+    <t xml:space="preserve">Emtricitabine and tenofovir alafenamide</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR20</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir alafenamide and bictegravir</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir alafenamide and bictegravir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR19</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir alafenamide and rilpivirine</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir alafenamide and rilpivirine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR22</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir alafenamide, darunavir and cobicistat</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir alafenamide, darunavir and cobicistat</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR18</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir alafenamide, elvitegravir and cobicistat</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir alafenamide, elvitegravir and cobicistat</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR06</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir disoproxil and efavirenz</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir disoproxil and efavirenz</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR08</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir disoproxil and rilpivirine</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir disoproxil and rilpivirine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR09</t>
   </si>
   <si>
-    <t xml:space="preserve">emtricitabine, tenofovir disoproxil, elvitegravir and cobicistat</t>
+    <t xml:space="preserve">Emtricitabine, tenofovir disoproxil, elvitegravir and cobicistat</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX07</t>
   </si>
   <si>
-    <t xml:space="preserve">enfuvirtide</t>
+    <t xml:space="preserve">Enfuvirtide</t>
   </si>
   <si>
     <t xml:space="preserve">c("Enfurvitide", "Enfuvirtide", "Fuzeon", "Pentafuside")</t>
@@ -347,16 +344,13 @@
     <t xml:space="preserve">J05AX17</t>
   </si>
   <si>
-    <t xml:space="preserve">enisamium iodide</t>
-  </si>
-  <si>
     <t xml:space="preserve">Enisamium iodide</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF10</t>
   </si>
   <si>
-    <t xml:space="preserve">entecavir</t>
+    <t xml:space="preserve">Entecavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Baraclude", "Entecavir", "Entecavir anhydrous", "Entecavirum")</t>
@@ -365,7 +359,7 @@
     <t xml:space="preserve">J05AG04</t>
   </si>
   <si>
-    <t xml:space="preserve">etravirine</t>
+    <t xml:space="preserve">Etravirine</t>
   </si>
   <si>
     <t xml:space="preserve">c("DAPY deriv", "Etravine", "Etravirine", "Intelence")</t>
@@ -374,16 +368,13 @@
     <t xml:space="preserve">J05AP04</t>
   </si>
   <si>
-    <t xml:space="preserve">faldaprevir</t>
-  </si>
-  <si>
     <t xml:space="preserve">Faldaprevir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB09</t>
   </si>
   <si>
-    <t xml:space="preserve">famciclovir</t>
+    <t xml:space="preserve">Famciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Famciclovir", "Famciclovirum", "Famvir", "Oravir")</t>
@@ -392,7 +383,7 @@
     <t xml:space="preserve">J05AE07</t>
   </si>
   <si>
-    <t xml:space="preserve">fosamprenavir</t>
+    <t xml:space="preserve">Fosamprenavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Amprenavir phosphate", "Fosamprenavir", "Lexiva", "Telzir")</t>
@@ -401,7 +392,7 @@
     <t xml:space="preserve">J05AD01</t>
   </si>
   <si>
-    <t xml:space="preserve">foscarnet</t>
+    <t xml:space="preserve">Foscarnet</t>
   </si>
   <si>
     <t xml:space="preserve">Phosphonic acid derivatives</t>
@@ -413,7 +404,7 @@
     <t xml:space="preserve">J05AD02</t>
   </si>
   <si>
-    <t xml:space="preserve">fosfonet</t>
+    <t xml:space="preserve">Fosfonet</t>
   </si>
   <si>
     <t xml:space="preserve">c("Fosfonet", "Fosfonet sodium", "Fosfonet Sodium", "Fosfonoacetate", "Fosfonoacetic acid", "Phosphonacetate", "Phosphonacetic acid")</t>
@@ -422,7 +413,7 @@
     <t xml:space="preserve">J05AB06</t>
   </si>
   <si>
-    <t xml:space="preserve">ganciclovir</t>
+    <t xml:space="preserve">Ganciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Citovirax", "Cymevan", "Cymeven", "Cymevene", "Cytovene", "Cytovene IV", "Ganciclovir", "Ganciclovirum", "Gancyclovir", "Hydroxyacyclovir", "Virgan", "Vitrasert", "Zirgan")</t>
@@ -431,19 +422,19 @@
     <t xml:space="preserve">J05AP57</t>
   </si>
   <si>
-    <t xml:space="preserve">glecaprevir and pibrentasvir</t>
+    <t xml:space="preserve">Glecaprevir and pibrentasvir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX23</t>
   </si>
   <si>
-    <t xml:space="preserve">ibalizumab</t>
+    <t xml:space="preserve">Ibalizumab</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB02</t>
   </si>
   <si>
-    <t xml:space="preserve">idoxuridine</t>
+    <t xml:space="preserve">Idoxuridine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Antizona", "Dendrid", "Emanil", "Heratil", "Herpesil", "Herpid", "Herpidu", "Herplex", "HERPLEX", "Herplex liquifilm", "Idexur", "Idossuridina", "Idoxene", "Idoxuridin", "Idoxuridina", "Idoxuridine", "Idoxuridinum", "Idu Oculos", "Iducher", "Idulea", "Iduoculos", "Iduridin", "Iduviran", "Iododeoxyridine", "Iododeoxyuridine", "Iodoxuridine", "Joddeoxiuridin", "Kerecid", "Kerecide", "Ophthalmadine", "Spectanefran", "Stoxil", "Synmiol", "Virudox")</t>
@@ -452,7 +443,7 @@
     <t xml:space="preserve">J05AE02</t>
   </si>
   <si>
-    <t xml:space="preserve">indinavir</t>
+    <t xml:space="preserve">Indinavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Compound J", "Crixivan", "Indinavir", "Indinavir anhydrous", "Propolis+Indinavir")</t>
@@ -461,7 +452,7 @@
     <t xml:space="preserve">J05AX05</t>
   </si>
   <si>
-    <t xml:space="preserve">inosine pranobex</t>
+    <t xml:space="preserve">Inosine pranobex</t>
   </si>
   <si>
     <t xml:space="preserve">c("Aviral", "Delimmun", "Immunovir", "Imunovir", "Inosine pranobex", "Inosiplex", "Isoprinosin", "Isoprinosina", "Isoprinosine", "Isoviral", "Methisoprinol", "Methysoprinol", "Metisoprinol", "Viruxan")</t>
@@ -470,7 +461,7 @@
     <t xml:space="preserve">J05AF05</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine</t>
+    <t xml:space="preserve">Lamivudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Epivir", "Hepitec", "Heptivir", "Heptodin", "Heptovir", "Lamivir", "Lamivudin", "Lamivudina", "Lamivudine", "Lamivudinum", "Zeffix")</t>
@@ -479,43 +470,43 @@
     <t xml:space="preserve">J05AR02</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine and abacavir</t>
+    <t xml:space="preserve">Lamivudine and abacavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR16</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine and raltegravir</t>
+    <t xml:space="preserve">Lamivudine and raltegravir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR12</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine and tenofovir disoproxil</t>
+    <t xml:space="preserve">Lamivudine and tenofovir disoproxil</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR13</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine, abacavir and dolutegravir</t>
+    <t xml:space="preserve">Lamivudine, abacavir and dolutegravir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR24</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine, tenofovir disoproxil and doravirine</t>
+    <t xml:space="preserve">Lamivudine, tenofovir disoproxil and doravirine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR11</t>
   </si>
   <si>
-    <t xml:space="preserve">lamivudine, tenofovir disoproxil and efavirenz</t>
+    <t xml:space="preserve">Lamivudine, tenofovir disoproxil and efavirenz</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX18</t>
   </si>
   <si>
-    <t xml:space="preserve">letermovir</t>
+    <t xml:space="preserve">Letermovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Letermovir", "Prevymis")</t>
@@ -524,7 +515,7 @@
     <t xml:space="preserve">J05AR10</t>
   </si>
   <si>
-    <t xml:space="preserve">lopinavir and ritonavir</t>
+    <t xml:space="preserve">Lopinavir and ritonavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Aluvia", "Kaletra")</t>
@@ -533,7 +524,7 @@
     <t xml:space="preserve">J05AX02</t>
   </si>
   <si>
-    <t xml:space="preserve">lysozyme</t>
+    <t xml:space="preserve">Lysozyme</t>
   </si>
   <si>
     <t xml:space="preserve">c("Lysozyme chloride", "Lysozyme Chloride", "Lysozyme G")</t>
@@ -542,7 +533,7 @@
     <t xml:space="preserve">J05AX09</t>
   </si>
   <si>
-    <t xml:space="preserve">maraviroc</t>
+    <t xml:space="preserve">Maraviroc</t>
   </si>
   <si>
     <t xml:space="preserve">c("Celsentri", "Maraviroc", "Selzentry")</t>
@@ -551,7 +542,7 @@
     <t xml:space="preserve">J05AX10</t>
   </si>
   <si>
-    <t xml:space="preserve">maribavir</t>
+    <t xml:space="preserve">Maribavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Benzimidavir", "Camvia", "Maribavir")</t>
@@ -560,7 +551,7 @@
     <t xml:space="preserve">J05AA01</t>
   </si>
   <si>
-    <t xml:space="preserve">metisazone</t>
+    <t xml:space="preserve">Metisazone</t>
   </si>
   <si>
     <t xml:space="preserve">Thiosemicarbazones</t>
@@ -572,7 +563,7 @@
     <t xml:space="preserve">J05AX01</t>
   </si>
   <si>
-    <t xml:space="preserve">moroxydine</t>
+    <t xml:space="preserve">Moroxydine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Bimolin", "Flumidine", "Influmine", "Moroxidina", "Moroxydine", "Moroxydinum", "Vironil", "Virugon", "Virumin", "Wirumin")</t>
@@ -581,7 +572,7 @@
     <t xml:space="preserve">J05AE04</t>
   </si>
   <si>
-    <t xml:space="preserve">nelfinavir</t>
+    <t xml:space="preserve">Nelfinavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Nelfinavir", "Viracept")</t>
@@ -590,7 +581,7 @@
     <t xml:space="preserve">J05AG01</t>
   </si>
   <si>
-    <t xml:space="preserve">nevirapine</t>
+    <t xml:space="preserve">Nevirapine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Nevirapine", "Nevirapine anhydrous", "Viramune", "Viramune IR", "Viramune XR")</t>
@@ -599,13 +590,13 @@
     <t xml:space="preserve">J05AP53</t>
   </si>
   <si>
-    <t xml:space="preserve">ombitasvir, paritaprevir and ritonavir</t>
+    <t xml:space="preserve">Ombitasvir, paritaprevir and ritonavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AH02</t>
   </si>
   <si>
-    <t xml:space="preserve">oseltamivir</t>
+    <t xml:space="preserve">Oseltamivir</t>
   </si>
   <si>
     <t xml:space="preserve">Neuraminidase inhibitors</t>
@@ -617,7 +608,7 @@
     <t xml:space="preserve">J05AB13</t>
   </si>
   <si>
-    <t xml:space="preserve">penciclovir</t>
+    <t xml:space="preserve">Penciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Adenovir", "Denavir", "Penciceovir", "Penciclovir", "Penciclovirum", "Pencyclovir", "Vectavir")</t>
@@ -626,7 +617,7 @@
     <t xml:space="preserve">J05AX21</t>
   </si>
   <si>
-    <t xml:space="preserve">pentanedioic acid imidazolyl ethanamide</t>
+    <t xml:space="preserve">Pentanedioic acid imidazolyl ethanamide</t>
   </si>
   <si>
     <t xml:space="preserve">Ingamine</t>
@@ -635,7 +626,7 @@
     <t xml:space="preserve">J05AH03</t>
   </si>
   <si>
-    <t xml:space="preserve">peramivir</t>
+    <t xml:space="preserve">Peramivir</t>
   </si>
   <si>
     <t xml:space="preserve">c("PeramiFlu", "Peramivir", "Rapiacta", "RAPIVAB")</t>
@@ -644,7 +635,7 @@
     <t xml:space="preserve">J05AX06</t>
   </si>
   <si>
-    <t xml:space="preserve">pleconaril</t>
+    <t xml:space="preserve">Pleconaril</t>
   </si>
   <si>
     <t xml:space="preserve">c("Picovir", "Pleconaril", "Pleconarilis")</t>
@@ -653,7 +644,7 @@
     <t xml:space="preserve">J05AX08</t>
   </si>
   <si>
-    <t xml:space="preserve">raltegravir</t>
+    <t xml:space="preserve">Raltegravir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Isentress", "Raltegravir")</t>
@@ -662,7 +653,7 @@
     <t xml:space="preserve">J05AP01</t>
   </si>
   <si>
-    <t xml:space="preserve">ribavirin</t>
+    <t xml:space="preserve">Ribavirin</t>
   </si>
   <si>
     <t xml:space="preserve">c("Copegus", "Cotronak", "Drug:  Ribavirin", "Ravanex", "Rebetol", "Rebetron", "Rebretron", "Ribacine", "Ribamide", "Ribamidil", "Ribamidyl", "Ribasphere", "Ribavirin", "Ribavirin Capsules", "Ribavirina", "Ribavirine", "Ribavirinum", "Ribovirin", "Tribavirin", "Varazid", "Vilona", "Viramid", "Viramide", "Virazid", "Virazide", "Virazole")</t>
@@ -671,7 +662,7 @@
     <t xml:space="preserve">J05AG05</t>
   </si>
   <si>
-    <t xml:space="preserve">rilpivirine</t>
+    <t xml:space="preserve">Rilpivirine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Edurant", "Rilpivirine")</t>
@@ -680,7 +671,7 @@
     <t xml:space="preserve">J05AC02</t>
   </si>
   <si>
-    <t xml:space="preserve">rimantadine</t>
+    <t xml:space="preserve">Rimantadine</t>
   </si>
   <si>
     <t xml:space="preserve">Cyclic amines</t>
@@ -692,7 +683,7 @@
     <t xml:space="preserve">J05AE03</t>
   </si>
   <si>
-    <t xml:space="preserve">ritonavir</t>
+    <t xml:space="preserve">Ritonavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Norvir", "Norvir Sec", "Norvir Softgel", "Ritonavir", "Ritonavire", "Ritonavirum")</t>
@@ -701,7 +692,7 @@
     <t xml:space="preserve">J05AE01</t>
   </si>
   <si>
-    <t xml:space="preserve">saquinavir</t>
+    <t xml:space="preserve">Saquinavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Fortovase", "Invirase", "Saquinavir")</t>
@@ -710,7 +701,7 @@
     <t xml:space="preserve">J05AP05</t>
   </si>
   <si>
-    <t xml:space="preserve">simeprevir</t>
+    <t xml:space="preserve">Simeprevir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Olysio", "Simeprevir sodium")</t>
@@ -719,7 +710,7 @@
     <t xml:space="preserve">J05AP08</t>
   </si>
   <si>
-    <t xml:space="preserve">sofosbuvir</t>
+    <t xml:space="preserve">Sofosbuvir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Hepcinat", "Hepcvir", "Sofosbuvir", "Sovaldi", "SOVALDI", "SoviHep")</t>
@@ -728,13 +719,13 @@
     <t xml:space="preserve">J05AP51</t>
   </si>
   <si>
-    <t xml:space="preserve">sofosbuvir and ledipasvir</t>
+    <t xml:space="preserve">Sofosbuvir and ledipasvir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP55</t>
   </si>
   <si>
-    <t xml:space="preserve">sofosbuvir and velpatasvir</t>
+    <t xml:space="preserve">Sofosbuvir and velpatasvir</t>
   </si>
   <si>
     <t xml:space="preserve">Epclusa Tablet</t>
@@ -743,13 +734,13 @@
     <t xml:space="preserve">J05AP56</t>
   </si>
   <si>
-    <t xml:space="preserve">sofosbuvir, velpatasvir and voxilaprevir</t>
+    <t xml:space="preserve">Sofosbuvir, velpatasvir and voxilaprevir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF04</t>
   </si>
   <si>
-    <t xml:space="preserve">stavudine</t>
+    <t xml:space="preserve">Stavudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Estavudina", "Sanilvudine", "Stavudin", "Stavudine", "Stavudinum", "Zerit Xr", "Zerut XR")</t>
@@ -758,7 +749,7 @@
     <t xml:space="preserve">J05AR07</t>
   </si>
   <si>
-    <t xml:space="preserve">stavudine, lamivudine and nevirapine</t>
+    <t xml:space="preserve">Stavudine, lamivudine and nevirapine</t>
   </si>
   <si>
     <t xml:space="preserve">STAVUDIINE</t>
@@ -767,7 +758,7 @@
     <t xml:space="preserve">J05AP02</t>
   </si>
   <si>
-    <t xml:space="preserve">telaprevir</t>
+    <t xml:space="preserve">Telaprevir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Incivek", "Incivo", "Telaprevir", "Telavic")</t>
@@ -776,7 +767,7 @@
     <t xml:space="preserve">J05AF11</t>
   </si>
   <si>
-    <t xml:space="preserve">telbivudine</t>
+    <t xml:space="preserve">Telbivudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Epavudine", "Sebivo", "Telbivudin", "Telbivudine", "Tyzeka")</t>
@@ -785,7 +776,7 @@
     <t xml:space="preserve">J05AF13</t>
   </si>
   <si>
-    <t xml:space="preserve">tenofovir alafenamide</t>
+    <t xml:space="preserve">Tenofovir alafenamide</t>
   </si>
   <si>
     <t xml:space="preserve">Vemlidy</t>
@@ -794,7 +785,7 @@
     <t xml:space="preserve">J05AF07</t>
   </si>
   <si>
-    <t xml:space="preserve">tenofovir disoproxil</t>
+    <t xml:space="preserve">Tenofovir disoproxil</t>
   </si>
   <si>
     <t xml:space="preserve">c("BisPMPA", "PMPA prodrug", "Tenofovir", "Viread")</t>
@@ -803,13 +794,13 @@
     <t xml:space="preserve">J05AR03</t>
   </si>
   <si>
-    <t xml:space="preserve">tenofovir disoproxil and emtricitabine</t>
+    <t xml:space="preserve">Tenofovir disoproxil and emtricitabine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX19</t>
   </si>
   <si>
-    <t xml:space="preserve">tilorone</t>
+    <t xml:space="preserve">Tilorone</t>
   </si>
   <si>
     <t xml:space="preserve">c("Amiksin", "Amixin", "Amixin IC", "Amyxin", "Tiloron", "Tilorona", "Tilorone", "Tiloronum")</t>
@@ -818,7 +809,7 @@
     <t xml:space="preserve">J05AE09</t>
   </si>
   <si>
-    <t xml:space="preserve">tipranavir</t>
+    <t xml:space="preserve">Tipranavir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Aptivus", "Tipranavir")</t>
@@ -827,7 +818,7 @@
     <t xml:space="preserve">J05AC03</t>
   </si>
   <si>
-    <t xml:space="preserve">tromantadine</t>
+    <t xml:space="preserve">Tromantadine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Tromantadina", "Tromantadine", "Tromantadinum", "Viruserol")</t>
@@ -836,7 +827,7 @@
     <t xml:space="preserve">J05AX13</t>
   </si>
   <si>
-    <t xml:space="preserve">umifenovir</t>
+    <t xml:space="preserve">Umifenovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Arbidol", "Arbidol base", "Umifenovir")</t>
@@ -845,7 +836,7 @@
     <t xml:space="preserve">J05AB11</t>
   </si>
   <si>
-    <t xml:space="preserve">valaciclovir</t>
+    <t xml:space="preserve">Valaciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Talavir", "Valaciclovir", "Valaciclovirum", "ValACV", "Valcivir", "Valcyclovir", "Valtrex", "Virval", "Zelitrex")</t>
@@ -854,7 +845,7 @@
     <t xml:space="preserve">J05AB14</t>
   </si>
   <si>
-    <t xml:space="preserve">valganciclovir</t>
+    <t xml:space="preserve">Valganciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">c("Cymeval", "Valganciclovir")</t>
@@ -863,7 +854,7 @@
     <t xml:space="preserve">J05AB03</t>
   </si>
   <si>
-    <t xml:space="preserve">vidarabine</t>
+    <t xml:space="preserve">Vidarabine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Adenine arabinoside", "Araadenosine", "Arabinoside adenine", "Arabinosyl adenine", "Arabinosyladenine", "Spongoadenosine", "Vidarabin", "Vidarabina", "Vidarabine", "Vidarabine anhydrous", "Vidarabinum", "Vira A", "Vira ATM")</t>
@@ -872,7 +863,7 @@
     <t xml:space="preserve">J05AF03</t>
   </si>
   <si>
-    <t xml:space="preserve">zalcitabine</t>
+    <t xml:space="preserve">Zalcitabine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Dideoxycytidine", "Interferon AD + ddC", "Zalcitabine", "Zalcitibine")</t>
@@ -881,7 +872,7 @@
     <t xml:space="preserve">J05AH01</t>
   </si>
   <si>
-    <t xml:space="preserve">zanamivir</t>
+    <t xml:space="preserve">Zanamivir</t>
   </si>
   <si>
     <t xml:space="preserve">c("MODIFIED SIALIC ACID", "Relenza", "Zanamavir", "Zanamir", "Zanamivi", "Zanamivir", "Zanamivir hydrate")</t>
@@ -890,7 +881,7 @@
     <t xml:space="preserve">J05AF01</t>
   </si>
   <si>
-    <t xml:space="preserve">zidovudine</t>
+    <t xml:space="preserve">Zidovudine</t>
   </si>
   <si>
     <t xml:space="preserve">c("Azidothymidine", "AZT Antiviral", "Beta interferon", "Compound S", "Propolis+AZT", "Retrovir", "Zidovudina", "Zidovudine", "ZIDOVUDINE", "Zidovudine EP III", "Zidovudinum")</t>
@@ -899,19 +890,19 @@
     <t xml:space="preserve">J05AR01</t>
   </si>
   <si>
-    <t xml:space="preserve">zidovudine and lamivudine</t>
+    <t xml:space="preserve">Zidovudine and lamivudine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR04</t>
   </si>
   <si>
-    <t xml:space="preserve">zidovudine, lamivudine and abacavir</t>
+    <t xml:space="preserve">Zidovudine, lamivudine and abacavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR05</t>
   </si>
   <si>
-    <t xml:space="preserve">zidovudine, lamivudine and nevirapine</t>
+    <t xml:space="preserve">Zidovudine, lamivudine and nevirapine</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1640,7 @@
         <v>28</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" t="n">
         <v>0.5</v>
@@ -1662,11 +1653,11 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>28</v>
@@ -1681,19 +1672,19 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="n">
         <v>5625</v>
       </c>
       <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
         <v>65</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>66</v>
-      </c>
-      <c r="E19" t="s">
-        <v>67</v>
       </c>
       <c r="F19" t="n">
         <v>1.2</v>
@@ -1706,19 +1697,19 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="n">
         <v>135398739</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" t="n">
         <v>0.4</v>
@@ -1731,19 +1722,19 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" t="n">
         <v>54726191</v>
       </c>
       <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
         <v>72</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>73</v>
-      </c>
-      <c r="E21" t="s">
-        <v>74</v>
       </c>
       <c r="F21" t="n">
         <v>50</v>
@@ -1756,13 +1747,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" t="n">
         <v>131801472</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
@@ -1777,19 +1768,19 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" t="n">
         <v>58460047</v>
       </c>
       <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
         <v>78</v>
-      </c>
-      <c r="D23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" t="s">
-        <v>79</v>
       </c>
       <c r="F23"/>
       <c r="G23"/>
@@ -1798,19 +1789,19 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" t="n">
         <v>64139</v>
       </c>
       <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
         <v>81</v>
-      </c>
-      <c r="D24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" t="s">
-        <v>82</v>
       </c>
       <c r="F24" t="n">
         <v>0.6</v>
@@ -1823,13 +1814,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B25" t="n">
         <v>91669168</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
         <v>28</v>
@@ -1844,19 +1835,19 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" t="n">
         <v>5277135</v>
       </c>
       <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
         <v>86</v>
-      </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>87</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
@@ -1865,19 +1856,19 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" t="n">
         <v>60877</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" t="n">
         <v>0.2</v>
@@ -1890,13 +1881,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" t="n">
         <v>90469070</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
@@ -1911,11 +1902,11 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29"/>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
@@ -1930,11 +1921,11 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30"/>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
         <v>35</v>
@@ -1949,11 +1940,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B31"/>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
         <v>35</v>
@@ -1968,11 +1959,11 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B32"/>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
         <v>35</v>
@@ -1987,11 +1978,11 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B33"/>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -2006,11 +1997,11 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34"/>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" t="s">
         <v>35</v>
@@ -2025,11 +2016,11 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35"/>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -2044,19 +2035,19 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B36" t="n">
         <v>16130199</v>
       </c>
       <c r="C36" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" t="s">
         <v>108</v>
-      </c>
-      <c r="D36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" t="s">
-        <v>109</v>
       </c>
       <c r="F36"/>
       <c r="G36"/>
@@ -2069,19 +2060,19 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="n">
         <v>10089466</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F37" t="n">
         <v>1.5</v>
@@ -2094,19 +2085,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B38" t="n">
         <v>135398508</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F38" t="n">
         <v>0.5</v>
@@ -2119,19 +2110,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B39" t="n">
         <v>193962</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F39" t="n">
         <v>0.4</v>
@@ -2144,19 +2135,19 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B40" t="n">
         <v>42601552</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F40"/>
       <c r="G40"/>
@@ -2165,19 +2156,19 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B41" t="n">
         <v>3324</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
         <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F41" t="n">
         <v>0.75</v>
@@ -2190,19 +2181,19 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B42" t="n">
         <v>131536</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D42" t="s">
         <v>24</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F42" t="n">
         <v>1.4</v>
@@ -2215,19 +2206,19 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B43" t="n">
         <v>3415</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F43"/>
       <c r="G43"/>
@@ -2240,19 +2231,19 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B44" t="n">
         <v>546</v>
       </c>
       <c r="C44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F44"/>
       <c r="G44"/>
@@ -2261,19 +2252,19 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B45" t="n">
         <v>135398740</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D45" t="s">
         <v>16</v>
       </c>
       <c r="E45" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F45" t="n">
         <v>3</v>
@@ -2290,11 +2281,11 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B46"/>
       <c r="C46" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
         <v>28</v>
@@ -2309,14 +2300,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B47"/>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" t="s">
         <v>36</v>
@@ -2328,19 +2319,19 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B48" t="n">
         <v>5905</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
         <v>16</v>
       </c>
       <c r="E48" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F48"/>
       <c r="G48"/>
@@ -2349,19 +2340,19 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B49" t="n">
         <v>5362440</v>
       </c>
       <c r="C49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D49" t="s">
         <v>24</v>
       </c>
       <c r="E49" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F49" t="n">
         <v>2.4</v>
@@ -2374,19 +2365,19 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B50" t="n">
         <v>135449284</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F50" t="n">
         <v>3</v>
@@ -2399,19 +2390,19 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B51" t="n">
         <v>60825</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F51" t="n">
         <v>0.3</v>
@@ -2424,11 +2415,11 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B52"/>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
         <v>35</v>
@@ -2443,13 +2434,13 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B53" t="n">
         <v>73386700</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D53" t="s">
         <v>35</v>
@@ -2464,11 +2455,11 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B54"/>
       <c r="C54" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D54" t="s">
         <v>35</v>
@@ -2483,11 +2474,11 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B55"/>
       <c r="C55" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D55" t="s">
         <v>35</v>
@@ -2502,11 +2493,11 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B56"/>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D56" t="s">
         <v>35</v>
@@ -2521,11 +2512,11 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B57"/>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D57" t="s">
         <v>35</v>
@@ -2540,19 +2531,19 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B58" t="n">
         <v>45138674</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F58" t="n">
         <v>0.48</v>
@@ -2569,19 +2560,19 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B59" t="n">
         <v>11979606</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>
       </c>
       <c r="E59" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F59" t="n">
         <v>0.8</v>
@@ -2594,19 +2585,19 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B60" t="n">
         <v>24839946</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E60" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F60"/>
       <c r="G60"/>
@@ -2615,19 +2606,19 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B61" t="n">
         <v>3002977</v>
       </c>
       <c r="C61" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F61" t="n">
         <v>0.6</v>
@@ -2640,19 +2631,19 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B62" t="n">
         <v>471161</v>
       </c>
       <c r="C62" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E62" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F62"/>
       <c r="G62"/>
@@ -2661,19 +2652,19 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B63" t="n">
         <v>667492</v>
       </c>
       <c r="C63" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F63"/>
       <c r="G63"/>
@@ -2682,19 +2673,19 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B64" t="n">
         <v>71655</v>
       </c>
       <c r="C64" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E64" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F64" t="n">
         <v>0.3</v>
@@ -2707,19 +2698,19 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B65" t="n">
         <v>64143</v>
       </c>
       <c r="C65" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D65" t="s">
         <v>24</v>
       </c>
       <c r="E65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F65" t="n">
         <v>2.25</v>
@@ -2732,19 +2723,19 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B66" t="n">
         <v>4463</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F66" t="n">
         <v>0.4</v>
@@ -2757,11 +2748,11 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B67"/>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D67" t="s">
         <v>28</v>
@@ -2776,19 +2767,19 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B68" t="n">
         <v>65028</v>
       </c>
       <c r="C68" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D68" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E68" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F68" t="n">
         <v>0.15</v>
@@ -2801,19 +2792,19 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B69" t="n">
         <v>135398748</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D69" t="s">
         <v>16</v>
       </c>
       <c r="E69" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F69"/>
       <c r="G69"/>
@@ -2822,19 +2813,19 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B70" t="n">
         <v>9942657</v>
       </c>
       <c r="C70" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F70" t="n">
         <v>90</v>
@@ -2847,19 +2838,19 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B71" t="n">
         <v>154234</v>
       </c>
       <c r="C71" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D71" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E71" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F71"/>
       <c r="G71"/>
@@ -2868,19 +2859,19 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B72" t="n">
         <v>1684</v>
       </c>
       <c r="C72" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E72" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F72"/>
       <c r="G72"/>
@@ -2889,19 +2880,19 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B73" t="n">
         <v>54671008</v>
       </c>
       <c r="C73" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E73" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F73" t="n">
         <v>0.8</v>
@@ -2914,19 +2905,19 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B74" t="n">
         <v>37542</v>
       </c>
       <c r="C74" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
         <v>28</v>
       </c>
       <c r="E74" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F74" t="n">
         <v>1</v>
@@ -2939,19 +2930,19 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B75" t="n">
         <v>6451164</v>
       </c>
       <c r="C75" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F75" t="n">
         <v>25</v>
@@ -2964,19 +2955,19 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B76" t="n">
         <v>5071</v>
       </c>
       <c r="C76" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D76" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E76" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F76" t="n">
         <v>0.2</v>
@@ -2989,19 +2980,19 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B77" t="n">
         <v>392622</v>
       </c>
       <c r="C77" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D77" t="s">
         <v>24</v>
       </c>
       <c r="E77" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F77" t="n">
         <v>1.2</v>
@@ -3014,19 +3005,19 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B78" t="n">
         <v>441243</v>
       </c>
       <c r="C78" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D78" t="s">
         <v>24</v>
       </c>
       <c r="E78" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F78" t="n">
         <v>1.8</v>
@@ -3039,19 +3030,19 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B79" t="n">
         <v>24873435</v>
       </c>
       <c r="C79" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D79" t="s">
         <v>28</v>
       </c>
       <c r="E79" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F79" t="n">
         <v>0.15</v>
@@ -3064,19 +3055,19 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B80" t="n">
         <v>45375808</v>
       </c>
       <c r="C80" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D80" t="s">
         <v>28</v>
       </c>
       <c r="E80" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F80" t="n">
         <v>0.4</v>
@@ -3089,13 +3080,13 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B81" t="n">
         <v>72734365</v>
       </c>
       <c r="C81" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D81" t="s">
         <v>28</v>
@@ -3110,19 +3101,19 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B82" t="n">
         <v>91885554</v>
       </c>
       <c r="C82" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D82" t="s">
         <v>28</v>
       </c>
       <c r="E82" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F82"/>
       <c r="G82"/>
@@ -3131,11 +3122,11 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B83"/>
       <c r="C83" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D83" t="s">
         <v>28</v>
@@ -3150,19 +3141,19 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B84" t="n">
         <v>18283</v>
       </c>
       <c r="C84" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
       </c>
       <c r="E84" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F84" t="n">
         <v>80</v>
@@ -3175,19 +3166,19 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B85" t="n">
         <v>15979285</v>
       </c>
       <c r="C85" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D85" t="s">
         <v>35</v>
       </c>
       <c r="E85" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F85"/>
       <c r="G85"/>
@@ -3196,19 +3187,19 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B86" t="n">
         <v>3010818</v>
       </c>
       <c r="C86" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D86" t="s">
         <v>28</v>
       </c>
       <c r="E86" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F86" t="n">
         <v>2.25</v>
@@ -3221,19 +3212,19 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B87" t="n">
         <v>159269</v>
       </c>
       <c r="C87" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D87" t="s">
         <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F87" t="n">
         <v>0.6</v>
@@ -3246,19 +3237,19 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B88" t="n">
         <v>9574768</v>
       </c>
       <c r="C88" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D88" t="s">
         <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F88" t="n">
         <v>25</v>
@@ -3271,19 +3262,19 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B89" t="n">
         <v>5481350</v>
       </c>
       <c r="C89" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
       </c>
       <c r="E89" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F89" t="n">
         <v>0.245</v>
@@ -3296,11 +3287,11 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B90"/>
       <c r="C90" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D90" t="s">
         <v>35</v>
@@ -3315,19 +3306,19 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B91" t="n">
         <v>5475</v>
       </c>
       <c r="C91" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E91" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F91" t="n">
         <v>0.125</v>
@@ -3340,19 +3331,19 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B92" t="n">
         <v>54682461</v>
       </c>
       <c r="C92" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D92" t="s">
         <v>24</v>
       </c>
       <c r="E92" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F92" t="n">
         <v>1</v>
@@ -3365,19 +3356,19 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B93" t="n">
         <v>64377</v>
       </c>
       <c r="C93" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D93" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F93"/>
       <c r="G93"/>
@@ -3386,19 +3377,19 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B94" t="n">
         <v>131411</v>
       </c>
       <c r="C94" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D94" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E94" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F94" t="n">
         <v>0.8</v>
@@ -3411,19 +3402,19 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B95" t="n">
         <v>135398742</v>
       </c>
       <c r="C95" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D95" t="s">
         <v>16</v>
       </c>
       <c r="E95" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F95" t="n">
         <v>3</v>
@@ -3436,19 +3427,19 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B96" t="n">
         <v>135413535</v>
       </c>
       <c r="C96" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D96" t="s">
         <v>16</v>
       </c>
       <c r="E96" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F96" t="n">
         <v>0.9</v>
@@ -3461,19 +3452,19 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B97" t="n">
         <v>21704</v>
       </c>
       <c r="C97" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D97" t="s">
         <v>16</v>
       </c>
       <c r="E97" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F97"/>
       <c r="G97"/>
@@ -3482,19 +3473,19 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B98" t="n">
         <v>24066</v>
       </c>
       <c r="C98" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D98" t="s">
         <v>11</v>
       </c>
       <c r="E98" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F98" t="n">
         <v>2.25</v>
@@ -3507,19 +3498,19 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B99" t="n">
         <v>60855</v>
       </c>
       <c r="C99" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D99" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E99" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F99"/>
       <c r="G99"/>
@@ -3528,19 +3519,19 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B100" t="n">
         <v>35370</v>
       </c>
       <c r="C100" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D100" t="s">
         <v>11</v>
       </c>
       <c r="E100" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F100" t="n">
         <v>0.6</v>
@@ -3557,11 +3548,11 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B101"/>
       <c r="C101" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D101" t="s">
         <v>35</v>
@@ -3576,11 +3567,11 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B102"/>
       <c r="C102" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D102" t="s">
         <v>35</v>
@@ -3595,11 +3586,11 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B103"/>
       <c r="C103" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D103" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
fix export of lists in `antibiotics` and `antivirals`
</commit_message>
<xml_diff>
--- a/data-raw/antivirals.xlsx
+++ b/data-raw/antivirals.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">Nucleoside and nucleotide reverse transcriptase inhibitors</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Abacavir", "Abacavir sulfate", "Ziagen")</t>
+    <t xml:space="preserve">Abacavir,Abacavir sulfate,Ziagen</t>
   </si>
   <si>
     <t xml:space="preserve">g</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Nucleosides and nucleotides excl. reverse transcriptase inhibitors</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Acicloftal", "Aciclovier", "Aciclovir", "Aciclovirum", "Activir", "AcycloFoam", "Acycloguanosine", "Acyclovir", "Acyclovir Lauriad", "ACYCLOVIR SODIUM", "Avirax", "Cargosil", "Cyclovir", "Genvir", "Gerpevir", "Hascovir", "Herpevir", "Maynar", "Poviral", "Sitavig", "Sitavir", "Vipral", "Virolex", "Viropump", "Virorax", "Zovirax", "Zovirax topical", "Zyclir")</t>
+    <t xml:space="preserve">Acicloftal,Aciclovier,Aciclovir,Aciclovirum,Activir,AcycloFoam,Acycloguanosine,Acyclovir,Acyclovir Lauriad,ACYCLOVIR SODIUM,Avirax,Cargosil,Cyclovir,Genvir,Gerpevir,Hascovir,Herpevir,Maynar,Poviral,Sitavig,Sitavir,Vipral,Virolex,Viropump,Virorax,Zovirax,Zovirax topical,Zyclir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF08</t>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Adefovir dipivoxil</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Adefovir di ester", "Adefovir dipivoxil", "Adefovir Dipivoxil", "Adefovir dipivoxyl", "Adefovir pivoxil", "Adefovirdipivoxl", "Bisadenine", "BISADENINE", "BisPMEA", "Hepsera", "Preveon", "YouHeDing")</t>
+    <t xml:space="preserve">Adefovir di ester,Adefovir dipivoxil,Adefovir Dipivoxil,Adefovir dipivoxyl,Adefovir pivoxil,Adefovirdipivoxl,Bisadenine,BISADENINE,BisPMEA,Hepsera,Preveon,YouHeDing</t>
   </si>
   <si>
     <t xml:space="preserve">mg</t>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">Protease inhibitors</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Agenerase", "Amprenavir", "Amprenavirum", "Prozei", "Vertex")</t>
+    <t xml:space="preserve">Agenerase,Amprenavir,Amprenavirum,Prozei,Vertex</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP06</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Antivirals for treatment of HCV infections</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Asunaprevir", "Sunvepra")</t>
+    <t xml:space="preserve">Asunaprevir,Sunvepra</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE08</t>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Atazanavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Atazanavir", "Atazanavir Base", "Latazanavir", "Reyataz", "Zrivada")</t>
+    <t xml:space="preserve">Atazanavir,Atazanavir Base,Latazanavir,Reyataz,Zrivada</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR15</t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">Boceprevir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Bocepravir", "Boceprevir", "Victrelis")</t>
+    <t xml:space="preserve">Bocepravir,Boceprevir,Victrelis</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB15</t>
@@ -146,7 +146,7 @@
     <t xml:space="preserve">Brivudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Bridic", "Brivox", "Brivudin", "Brivudina", "Brivudine", "Brivudinum", "BrVdUrd", "Helpin", "Zerpex", "Zostex")</t>
+    <t xml:space="preserve">Bridic,Brivox,Brivudin,Brivudina,Brivudine,Brivudinum,BrVdUrd,Helpin,Zerpex,Zostex</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB12</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">Cidofovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Cidofovir", "Cidofovir anhydrous", "Cidofovir gel", "Cidofovirum", "Forvade", "Vistide")</t>
+    <t xml:space="preserve">Cidofovir,Cidofovir anhydrous,Cidofovir gel,Cidofovirum,Forvade,Vistide</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF12</t>
@@ -164,7 +164,7 @@
     <t xml:space="preserve">Clevudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Clevudine", "Levovir", "Revovir")</t>
+    <t xml:space="preserve">Clevudine,Levovir,Revovir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP07</t>
@@ -173,7 +173,7 @@
     <t xml:space="preserve">Daclatasvir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Daclatasvir", "Daklinza")</t>
+    <t xml:space="preserve">Daclatasvir,Daklinza</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE10</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">Darunavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Darunavir", "Darunavirum", "Prezista", "Prezista Naive")</t>
+    <t xml:space="preserve">Darunavir,Darunavirum,Prezista,Prezista Naive</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR14</t>
@@ -212,7 +212,7 @@
     <t xml:space="preserve">Non-nucleoside reverse transcriptase inhibitors</t>
   </si>
   <si>
-    <t xml:space="preserve">c("BHAP der", "Delavirdin", "Delavirdina", "Delavirdine", "Delavirdinum", "PIPERAZINE", "Rescriptor")</t>
+    <t xml:space="preserve">BHAP der,Delavirdin,Delavirdina,Delavirdine,Delavirdinum,PIPERAZINE,Rescriptor</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF02</t>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">Didanosine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Didanosina", "Didanosine", "Didanosinum", "Dideoxyinosine", "DIDEOXYINOSINE", "Hypoxanthine ddN", "Videx", "Videx EC")</t>
+    <t xml:space="preserve">Didanosina,Didanosine,Didanosinum,Dideoxyinosine,DIDEOXYINOSINE,Hypoxanthine ddN,Videx,Videx EC</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX12</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Other antivirals</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Dolutegravir", "Dolutegravir Sodium", "Soltegravir", "Tivicay")</t>
+    <t xml:space="preserve">Dolutegravir,Dolutegravir Sodium,Soltegravir,Tivicay</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR21</t>
@@ -248,7 +248,7 @@
     <t xml:space="preserve">Doravirine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Doravirine", "Pifeltro")</t>
+    <t xml:space="preserve">Doravirine,Pifeltro</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG03</t>
@@ -257,7 +257,7 @@
     <t xml:space="preserve">Efavirenz</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Efavirenz", "Efavirenzum", "Eravirenz", "Stocrin", "Strocin", "Sustiva")</t>
+    <t xml:space="preserve">Efavirenz,Efavirenzum,Eravirenz,Stocrin,Strocin,Sustiva</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP54</t>
@@ -272,7 +272,7 @@
     <t xml:space="preserve">Elvitegravir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Elvitegravir", "Vitekta")</t>
+    <t xml:space="preserve">Elvitegravir,Vitekta</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF09</t>
@@ -281,7 +281,7 @@
     <t xml:space="preserve">Emtricitabine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Coviracil", "Emtricitabin", "Emtricitabina", "Emtricitabine", "Emtricitabinum", "Emtritabine", "Emtriva", "Racivir")</t>
+    <t xml:space="preserve">Coviracil,Emtricitabin,Emtricitabina,Emtricitabine,Emtricitabinum,Emtritabine,Emtriva,Racivir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR17</t>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">Enfuvirtide</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Enfurvitide", "Enfuvirtide", "Fuzeon", "Pentafuside")</t>
+    <t xml:space="preserve">Enfurvitide,Enfuvirtide,Fuzeon,Pentafuside</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX17</t>
@@ -353,7 +353,7 @@
     <t xml:space="preserve">Entecavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Baraclude", "Entecavir", "Entecavir anhydrous", "Entecavirum")</t>
+    <t xml:space="preserve">Baraclude,Entecavir,Entecavir anhydrous,Entecavirum</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG04</t>
@@ -362,7 +362,7 @@
     <t xml:space="preserve">Etravirine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("DAPY deriv", "Etravine", "Etravirine", "Intelence")</t>
+    <t xml:space="preserve">DAPY deriv,Etravine,Etravirine,Intelence</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP04</t>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">Famciclovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Famciclovir", "Famciclovirum", "Famvir", "Oravir")</t>
+    <t xml:space="preserve">Famciclovir,Famciclovirum,Famvir,Oravir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE07</t>
@@ -386,7 +386,7 @@
     <t xml:space="preserve">Fosamprenavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Amprenavir phosphate", "Fosamprenavir", "Lexiva", "Telzir")</t>
+    <t xml:space="preserve">Amprenavir phosphate,Fosamprenavir,Lexiva,Telzir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AD01</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Phosphonic acid derivatives</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Forscarnet", "Forscarnet sodium", "Foscarmet", "Foscarnet", "Phosphonoformate", "Phosphonoformic acid")</t>
+    <t xml:space="preserve">Forscarnet,Forscarnet sodium,Foscarmet,Foscarnet,Phosphonoformate,Phosphonoformic acid</t>
   </si>
   <si>
     <t xml:space="preserve">J05AD02</t>
@@ -407,7 +407,7 @@
     <t xml:space="preserve">Fosfonet</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Fosfonet", "Fosfonet sodium", "Fosfonet Sodium", "Fosfonoacetate", "Fosfonoacetic acid", "Phosphonacetate", "Phosphonacetic acid")</t>
+    <t xml:space="preserve">Fosfonet,Fosfonet sodium,Fosfonet Sodium,Fosfonoacetate,Fosfonoacetic acid,Phosphonacetate,Phosphonacetic acid</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB06</t>
@@ -416,7 +416,7 @@
     <t xml:space="preserve">Ganciclovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Citovirax", "Cymevan", "Cymeven", "Cymevene", "Cytovene", "Cytovene IV", "Ganciclovir", "Ganciclovirum", "Gancyclovir", "Hydroxyacyclovir", "Virgan", "Vitrasert", "Zirgan")</t>
+    <t xml:space="preserve">Citovirax,Cymevan,Cymeven,Cymevene,Cytovene,Cytovene IV,Ganciclovir,Ganciclovirum,Gancyclovir,Hydroxyacyclovir,Virgan,Vitrasert,Zirgan</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP57</t>
@@ -437,7 +437,7 @@
     <t xml:space="preserve">Idoxuridine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Antizona", "Dendrid", "Emanil", "Heratil", "Herpesil", "Herpid", "Herpidu", "Herplex", "HERPLEX", "Herplex liquifilm", "Idexur", "Idossuridina", "Idoxene", "Idoxuridin", "Idoxuridina", "Idoxuridine", "Idoxuridinum", "Idu Oculos", "Iducher", "Idulea", "Iduoculos", "Iduridin", "Iduviran", "Iododeoxyridine", "Iododeoxyuridine", "Iodoxuridine", "Joddeoxiuridin", "Kerecid", "Kerecide", "Ophthalmadine", "Spectanefran", "Stoxil", "Synmiol", "Virudox")</t>
+    <t xml:space="preserve">Antizona,Dendrid,Emanil,Heratil,Herpesil,Herpid,Herpidu,Herplex,HERPLEX,Herplex liquifilm,Idexur,Idossuridina,Idoxene,Idoxuridin,Idoxuridina,Idoxuridine,Idoxuridinum,Idu Oculos,Iducher,Idulea,Iduoculos,Iduridin,Iduviran,Iododeoxyridine,Iododeoxyuridine,Iodoxuridine,Joddeoxiuridin,Kerecid,Kerecide,Ophthalmadine,Spectanefran,Stoxil,Synmiol,Virudox</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE02</t>
@@ -446,7 +446,7 @@
     <t xml:space="preserve">Indinavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Compound J", "Crixivan", "Indinavir", "Indinavir anhydrous", "Propolis+Indinavir")</t>
+    <t xml:space="preserve">Compound J,Crixivan,Indinavir,Indinavir anhydrous,Propolis+Indinavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX05</t>
@@ -455,7 +455,7 @@
     <t xml:space="preserve">Inosine pranobex</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Aviral", "Delimmun", "Immunovir", "Imunovir", "Inosine pranobex", "Inosiplex", "Isoprinosin", "Isoprinosina", "Isoprinosine", "Isoviral", "Methisoprinol", "Methysoprinol", "Metisoprinol", "Viruxan")</t>
+    <t xml:space="preserve">Aviral,Delimmun,Immunovir,Imunovir,Inosine pranobex,Inosiplex,Isoprinosin,Isoprinosina,Isoprinosine,Isoviral,Methisoprinol,Methysoprinol,Metisoprinol,Viruxan</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF05</t>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">Lamivudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Epivir", "Hepitec", "Heptivir", "Heptodin", "Heptovir", "Lamivir", "Lamivudin", "Lamivudina", "Lamivudine", "Lamivudinum", "Zeffix")</t>
+    <t xml:space="preserve">Epivir,Hepitec,Heptivir,Heptodin,Heptovir,Lamivir,Lamivudin,Lamivudina,Lamivudine,Lamivudinum,Zeffix</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR02</t>
@@ -509,7 +509,7 @@
     <t xml:space="preserve">Letermovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Letermovir", "Prevymis")</t>
+    <t xml:space="preserve">Letermovir,Prevymis</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR10</t>
@@ -518,7 +518,7 @@
     <t xml:space="preserve">Lopinavir and ritonavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Aluvia", "Kaletra")</t>
+    <t xml:space="preserve">Aluvia,Kaletra</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX02</t>
@@ -527,7 +527,7 @@
     <t xml:space="preserve">Lysozyme</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Lysozyme chloride", "Lysozyme Chloride", "Lysozyme G")</t>
+    <t xml:space="preserve">Lysozyme chloride,Lysozyme Chloride,Lysozyme G</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX09</t>
@@ -536,7 +536,7 @@
     <t xml:space="preserve">Maraviroc</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Celsentri", "Maraviroc", "Selzentry")</t>
+    <t xml:space="preserve">Celsentri,Maraviroc,Selzentry</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX10</t>
@@ -545,7 +545,7 @@
     <t xml:space="preserve">Maribavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Benzimidavir", "Camvia", "Maribavir")</t>
+    <t xml:space="preserve">Benzimidavir,Camvia,Maribavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AA01</t>
@@ -557,7 +557,7 @@
     <t xml:space="preserve">Thiosemicarbazones</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Kemoviran", "Marboran", "Marborane", "Methisazon", "Methisazone", "Methsazone", "Metisazon", "Metisazona", "Metisazone", "Metisazonum", "Viruzona")</t>
+    <t xml:space="preserve">Kemoviran,Marboran,Marborane,Methisazon,Methisazone,Methsazone,Metisazon,Metisazona,Metisazone,Metisazonum,Viruzona</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX01</t>
@@ -566,7 +566,7 @@
     <t xml:space="preserve">Moroxydine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Bimolin", "Flumidine", "Influmine", "Moroxidina", "Moroxydine", "Moroxydinum", "Vironil", "Virugon", "Virumin", "Wirumin")</t>
+    <t xml:space="preserve">Bimolin,Flumidine,Influmine,Moroxidina,Moroxydine,Moroxydinum,Vironil,Virugon,Virumin,Wirumin</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE04</t>
@@ -575,7 +575,7 @@
     <t xml:space="preserve">Nelfinavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Nelfinavir", "Viracept")</t>
+    <t xml:space="preserve">Nelfinavir,Viracept</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG01</t>
@@ -584,7 +584,7 @@
     <t xml:space="preserve">Nevirapine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Nevirapine", "Nevirapine anhydrous", "Viramune", "Viramune IR", "Viramune XR")</t>
+    <t xml:space="preserve">Nevirapine,Nevirapine anhydrous,Viramune,Viramune IR,Viramune XR</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP53</t>
@@ -602,7 +602,7 @@
     <t xml:space="preserve">Neuraminidase inhibitors</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Agucort", "Oseltamivir", "Tamiflu", "Tamvir")</t>
+    <t xml:space="preserve">Agucort,Oseltamivir,Tamiflu,Tamvir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB13</t>
@@ -611,7 +611,7 @@
     <t xml:space="preserve">Penciclovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Adenovir", "Denavir", "Penciceovir", "Penciclovir", "Penciclovirum", "Pencyclovir", "Vectavir")</t>
+    <t xml:space="preserve">Adenovir,Denavir,Penciceovir,Penciclovir,Penciclovirum,Pencyclovir,Vectavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX21</t>
@@ -629,7 +629,7 @@
     <t xml:space="preserve">Peramivir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("PeramiFlu", "Peramivir", "Rapiacta", "RAPIVAB")</t>
+    <t xml:space="preserve">PeramiFlu,Peramivir,Rapiacta,RAPIVAB</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX06</t>
@@ -638,7 +638,7 @@
     <t xml:space="preserve">Pleconaril</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Picovir", "Pleconaril", "Pleconarilis")</t>
+    <t xml:space="preserve">Picovir,Pleconaril,Pleconarilis</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX08</t>
@@ -647,7 +647,7 @@
     <t xml:space="preserve">Raltegravir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Isentress", "Raltegravir")</t>
+    <t xml:space="preserve">Isentress,Raltegravir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP01</t>
@@ -656,7 +656,7 @@
     <t xml:space="preserve">Ribavirin</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Copegus", "Cotronak", "Drug:  Ribavirin", "Ravanex", "Rebetol", "Rebetron", "Rebretron", "Ribacine", "Ribamide", "Ribamidil", "Ribamidyl", "Ribasphere", "Ribavirin", "Ribavirin Capsules", "Ribavirina", "Ribavirine", "Ribavirinum", "Ribovirin", "Tribavirin", "Varazid", "Vilona", "Viramid", "Viramide", "Virazid", "Virazide", "Virazole")</t>
+    <t xml:space="preserve">Copegus,Cotronak,Drug:  Ribavirin,Ravanex,Rebetol,Rebetron,Rebretron,Ribacine,Ribamide,Ribamidil,Ribamidyl,Ribasphere,Ribavirin,Ribavirin Capsules,Ribavirina,Ribavirine,Ribavirinum,Ribovirin,Tribavirin,Varazid,Vilona,Viramid,Viramide,Virazid,Virazide,Virazole</t>
   </si>
   <si>
     <t xml:space="preserve">J05AG05</t>
@@ -665,7 +665,7 @@
     <t xml:space="preserve">Rilpivirine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Edurant", "Rilpivirine")</t>
+    <t xml:space="preserve">Edurant,Rilpivirine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AC02</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">Cyclic amines</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Remantadine", "Riamantadine", "Rimant", "RIMANTADIN", "Rimantadin A", "Rimantadina", "Rimantadine", "Rimantadinum")</t>
+    <t xml:space="preserve">Remantadine,Riamantadine,Rimant,RIMANTADIN,Rimantadin A,Rimantadina,Rimantadine,Rimantadinum</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE03</t>
@@ -686,7 +686,7 @@
     <t xml:space="preserve">Ritonavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Norvir", "Norvir Sec", "Norvir Softgel", "Ritonavir", "Ritonavire", "Ritonavirum")</t>
+    <t xml:space="preserve">Norvir,Norvir Sec,Norvir Softgel,Ritonavir,Ritonavire,Ritonavirum</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE01</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">Saquinavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Fortovase", "Invirase", "Saquinavir")</t>
+    <t xml:space="preserve">Fortovase,Invirase,Saquinavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP05</t>
@@ -704,7 +704,7 @@
     <t xml:space="preserve">Simeprevir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Olysio", "Simeprevir sodium")</t>
+    <t xml:space="preserve">Olysio,Simeprevir sodium</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP08</t>
@@ -713,7 +713,7 @@
     <t xml:space="preserve">Sofosbuvir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Hepcinat", "Hepcvir", "Sofosbuvir", "Sovaldi", "SOVALDI", "SoviHep")</t>
+    <t xml:space="preserve">Hepcinat,Hepcvir,Sofosbuvir,Sovaldi,SOVALDI,SoviHep</t>
   </si>
   <si>
     <t xml:space="preserve">J05AP51</t>
@@ -743,7 +743,7 @@
     <t xml:space="preserve">Stavudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Estavudina", "Sanilvudine", "Stavudin", "Stavudine", "Stavudinum", "Zerit Xr", "Zerut XR")</t>
+    <t xml:space="preserve">Estavudina,Sanilvudine,Stavudin,Stavudine,Stavudinum,Zerit Xr,Zerut XR</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR07</t>
@@ -761,7 +761,7 @@
     <t xml:space="preserve">Telaprevir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Incivek", "Incivo", "Telaprevir", "Telavic")</t>
+    <t xml:space="preserve">Incivek,Incivo,Telaprevir,Telavic</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF11</t>
@@ -770,7 +770,7 @@
     <t xml:space="preserve">Telbivudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Epavudine", "Sebivo", "Telbivudin", "Telbivudine", "Tyzeka")</t>
+    <t xml:space="preserve">Epavudine,Sebivo,Telbivudin,Telbivudine,Tyzeka</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF13</t>
@@ -788,7 +788,7 @@
     <t xml:space="preserve">Tenofovir disoproxil</t>
   </si>
   <si>
-    <t xml:space="preserve">c("BisPMPA", "PMPA prodrug", "Tenofovir", "Viread")</t>
+    <t xml:space="preserve">BisPMPA,PMPA prodrug,Tenofovir,Viread</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR03</t>
@@ -803,7 +803,7 @@
     <t xml:space="preserve">Tilorone</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Amiksin", "Amixin", "Amixin IC", "Amyxin", "Tiloron", "Tilorona", "Tilorone", "Tiloronum")</t>
+    <t xml:space="preserve">Amiksin,Amixin,Amixin IC,Amyxin,Tiloron,Tilorona,Tilorone,Tiloronum</t>
   </si>
   <si>
     <t xml:space="preserve">J05AE09</t>
@@ -812,7 +812,7 @@
     <t xml:space="preserve">Tipranavir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Aptivus", "Tipranavir")</t>
+    <t xml:space="preserve">Aptivus,Tipranavir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AC03</t>
@@ -821,7 +821,7 @@
     <t xml:space="preserve">Tromantadine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Tromantadina", "Tromantadine", "Tromantadinum", "Viruserol")</t>
+    <t xml:space="preserve">Tromantadina,Tromantadine,Tromantadinum,Viruserol</t>
   </si>
   <si>
     <t xml:space="preserve">J05AX13</t>
@@ -830,7 +830,7 @@
     <t xml:space="preserve">Umifenovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Arbidol", "Arbidol base", "Umifenovir")</t>
+    <t xml:space="preserve">Arbidol,Arbidol base,Umifenovir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB11</t>
@@ -839,7 +839,7 @@
     <t xml:space="preserve">Valaciclovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Talavir", "Valaciclovir", "Valaciclovirum", "ValACV", "Valcivir", "Valcyclovir", "Valtrex", "Virval", "Zelitrex")</t>
+    <t xml:space="preserve">Talavir,Valaciclovir,Valaciclovirum,ValACV,Valcivir,Valcyclovir,Valtrex,Virval,Zelitrex</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB14</t>
@@ -848,7 +848,7 @@
     <t xml:space="preserve">Valganciclovir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Cymeval", "Valganciclovir")</t>
+    <t xml:space="preserve">Cymeval,Valganciclovir</t>
   </si>
   <si>
     <t xml:space="preserve">J05AB03</t>
@@ -857,7 +857,7 @@
     <t xml:space="preserve">Vidarabine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Adenine arabinoside", "Araadenosine", "Arabinoside adenine", "Arabinosyl adenine", "Arabinosyladenine", "Spongoadenosine", "Vidarabin", "Vidarabina", "Vidarabine", "Vidarabine anhydrous", "Vidarabinum", "Vira A", "Vira ATM")</t>
+    <t xml:space="preserve">Adenine arabinoside,Araadenosine,Arabinoside adenine,Arabinosyl adenine,Arabinosyladenine,Spongoadenosine,Vidarabin,Vidarabina,Vidarabine,Vidarabine anhydrous,Vidarabinum,Vira A,Vira ATM</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF03</t>
@@ -866,7 +866,7 @@
     <t xml:space="preserve">Zalcitabine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Dideoxycytidine", "Interferon AD + ddC", "Zalcitabine", "Zalcitibine")</t>
+    <t xml:space="preserve">Dideoxycytidine,Interferon AD + ddC,Zalcitabine,Zalcitibine</t>
   </si>
   <si>
     <t xml:space="preserve">J05AH01</t>
@@ -875,7 +875,7 @@
     <t xml:space="preserve">Zanamivir</t>
   </si>
   <si>
-    <t xml:space="preserve">c("MODIFIED SIALIC ACID", "Relenza", "Zanamavir", "Zanamir", "Zanamivi", "Zanamivir", "Zanamivir hydrate")</t>
+    <t xml:space="preserve">MODIFIED SIALIC ACID,Relenza,Zanamavir,Zanamir,Zanamivi,Zanamivir,Zanamivir hydrate</t>
   </si>
   <si>
     <t xml:space="preserve">J05AF01</t>
@@ -884,7 +884,7 @@
     <t xml:space="preserve">Zidovudine</t>
   </si>
   <si>
-    <t xml:space="preserve">c("Azidothymidine", "AZT Antiviral", "Beta interferon", "Compound S", "Propolis+AZT", "Retrovir", "Zidovudina", "Zidovudine", "ZIDOVUDINE", "Zidovudine EP III", "Zidovudinum")</t>
+    <t xml:space="preserve">Azidothymidine,AZT Antiviral,Beta interferon,Compound S,Propolis+AZT,Retrovir,Zidovudina,Zidovudine,ZIDOVUDINE,Zidovudine EP III,Zidovudinum</t>
   </si>
   <si>
     <t xml:space="preserve">J05AR01</t>

</xml_diff>